<commit_message>
Some fixes for running without timeseries reduction, added integration test
</commit_message>
<xml_diff>
--- a/data/output/results/Example_building_opt/InputData.xlsx
+++ b/data/output/results/Example_building_opt/InputData.xlsx
@@ -37,7 +37,7 @@
     <t>('SCENARIO VALUES', 'BAU')</t>
   </si>
   <si>
-    <t>('SCENARIO VALUES', 'PV + WP')</t>
+    <t>('SCENARIO VALUES', 'PV + HP')</t>
   </si>
   <si>
     <t>('SCENARIO VALUES', 'Refurbished')</t>
@@ -1393,58 +1393,58 @@
     <t>default 1000 kW, actual potential is calculated using the solar potential area (Building Data)</t>
   </si>
   <si>
-    <t>default 98%</t>
+    <t>default 96%</t>
+  </si>
+  <si>
+    <t>default 99.8% ~ 5% per day</t>
+  </si>
+  <si>
+    <t>typically 10 - 15a</t>
+  </si>
+  <si>
+    <t>default 3000</t>
+  </si>
+  <si>
+    <t>default 1</t>
+  </si>
+  <si>
+    <t>default 20%</t>
+  </si>
+  <si>
+    <t>typically around 500 - 1500€/kWh</t>
+  </si>
+  <si>
+    <t>default 230</t>
+  </si>
+  <si>
+    <t>most common: flatplate_singlecover_sel</t>
+  </si>
+  <si>
+    <t>default 100</t>
+  </si>
+  <si>
+    <t>specifications need to be given</t>
+  </si>
+  <si>
+    <t>typically 15 years</t>
+  </si>
+  <si>
+    <t>investment costs for heatpump itself</t>
+  </si>
+  <si>
+    <t>installation costs independent of HP size</t>
+  </si>
+  <si>
+    <t>costs for HP-ready retrofit</t>
+  </si>
+  <si>
+    <t>default 0</t>
+  </si>
+  <si>
+    <t>typicaly 15 years</t>
   </si>
   <si>
     <t>default 95%</t>
-  </si>
-  <si>
-    <t>default 99.99%</t>
-  </si>
-  <si>
-    <t>typically 10 - 15a</t>
-  </si>
-  <si>
-    <t>default 3000</t>
-  </si>
-  <si>
-    <t>default 1</t>
-  </si>
-  <si>
-    <t>default 20%</t>
-  </si>
-  <si>
-    <t>typically around 500 - 1500€/kWh</t>
-  </si>
-  <si>
-    <t>default 230</t>
-  </si>
-  <si>
-    <t>most common: flatplate_singlecover_sel</t>
-  </si>
-  <si>
-    <t>default 100</t>
-  </si>
-  <si>
-    <t>specifications need to be given</t>
-  </si>
-  <si>
-    <t>typically 15 years</t>
-  </si>
-  <si>
-    <t>investment costs for heatpump itself</t>
-  </si>
-  <si>
-    <t>installation costs independent of HP size</t>
-  </si>
-  <si>
-    <t>costs for HP-ready retrofit</t>
-  </si>
-  <si>
-    <t>default 0</t>
-  </si>
-  <si>
-    <t>typicaly 15 years</t>
   </si>
   <si>
     <t>default 99.5%</t>
@@ -6854,16 +6854,16 @@
         <v>18</v>
       </c>
       <c r="F46">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="G46">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="H46">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
       <c r="I46">
-        <v>0.98</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="47" spans="1:9">
@@ -6877,22 +6877,22 @@
         <v>435</v>
       </c>
       <c r="D47" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="E47" t="s">
         <v>18</v>
       </c>
       <c r="F47">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="G47">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="H47">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
       <c r="I47">
-        <v>0.95</v>
+        <v>0.96</v>
       </c>
     </row>
     <row r="48" spans="1:9">
@@ -6906,22 +6906,22 @@
         <v>435</v>
       </c>
       <c r="D48" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="E48" t="s">
         <v>18</v>
       </c>
       <c r="F48">
-        <v>0.9999</v>
+        <v>0.998</v>
       </c>
       <c r="G48">
-        <v>0.9999</v>
+        <v>0.998</v>
       </c>
       <c r="H48">
-        <v>0.9999</v>
+        <v>0.998</v>
       </c>
       <c r="I48">
-        <v>0.9999</v>
+        <v>0.998</v>
       </c>
     </row>
     <row r="49" spans="1:9">
@@ -6935,7 +6935,7 @@
         <v>436</v>
       </c>
       <c r="D49" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E49" t="s">
         <v>220</v>
@@ -6964,7 +6964,7 @@
         <v>84</v>
       </c>
       <c r="D50" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="E50" t="s">
         <v>18</v>
@@ -6993,7 +6993,7 @@
         <v>84</v>
       </c>
       <c r="D51" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E51" t="s">
         <v>18</v>
@@ -7022,7 +7022,7 @@
         <v>435</v>
       </c>
       <c r="D52" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E52" t="s">
         <v>18</v>
@@ -7051,7 +7051,7 @@
         <v>443</v>
       </c>
       <c r="D53" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="E53" t="s">
         <v>18</v>
@@ -7225,7 +7225,7 @@
         <v>444</v>
       </c>
       <c r="D59" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E59" t="s">
         <v>18</v>
@@ -7312,7 +7312,7 @@
         <v>16</v>
       </c>
       <c r="D62" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E62" t="s">
         <v>98</v>
@@ -7544,7 +7544,7 @@
         <v>445</v>
       </c>
       <c r="D70" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E70" t="s">
         <v>18</v>
@@ -7631,7 +7631,7 @@
         <v>16</v>
       </c>
       <c r="D73" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E73" t="s">
         <v>98</v>
@@ -7863,7 +7863,7 @@
         <v>445</v>
       </c>
       <c r="D81" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E81" t="s">
         <v>18</v>
@@ -7950,7 +7950,7 @@
         <v>16</v>
       </c>
       <c r="D84" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E84" t="s">
         <v>98</v>
@@ -8182,7 +8182,7 @@
         <v>445</v>
       </c>
       <c r="D92" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E92" t="s">
         <v>18</v>
@@ -8269,7 +8269,7 @@
         <v>16</v>
       </c>
       <c r="D95" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="E95" t="s">
         <v>98</v>
@@ -8501,7 +8501,7 @@
         <v>445</v>
       </c>
       <c r="D103" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="E103" t="s">
         <v>18</v>
@@ -8559,7 +8559,7 @@
         <v>84</v>
       </c>
       <c r="D105" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E105" t="s">
         <v>98</v>
@@ -8588,7 +8588,7 @@
         <v>436</v>
       </c>
       <c r="D106" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E106" t="s">
         <v>220</v>
@@ -8617,7 +8617,7 @@
         <v>443</v>
       </c>
       <c r="D107" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E107" t="s">
         <v>18</v>
@@ -8646,7 +8646,7 @@
         <v>438</v>
       </c>
       <c r="D108" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E108" t="s">
         <v>18</v>
@@ -8675,7 +8675,7 @@
         <v>439</v>
       </c>
       <c r="D109" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E109" t="s">
         <v>18</v>
@@ -8791,7 +8791,7 @@
         <v>446</v>
       </c>
       <c r="D113" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E113" t="s">
         <v>18</v>
@@ -8849,7 +8849,7 @@
         <v>84</v>
       </c>
       <c r="D115" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="E115" t="s">
         <v>98</v>
@@ -8878,7 +8878,7 @@
         <v>436</v>
       </c>
       <c r="D116" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="E116" t="s">
         <v>220</v>
@@ -8907,7 +8907,7 @@
         <v>443</v>
       </c>
       <c r="D117" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E117" t="s">
         <v>18</v>
@@ -8936,7 +8936,7 @@
         <v>438</v>
       </c>
       <c r="D118" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E118" t="s">
         <v>18</v>
@@ -8965,7 +8965,7 @@
         <v>439</v>
       </c>
       <c r="D119" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="E119" t="s">
         <v>18</v>
@@ -9081,7 +9081,7 @@
         <v>446</v>
       </c>
       <c r="D123" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E123" t="s">
         <v>18</v>
@@ -9168,7 +9168,7 @@
         <v>436</v>
       </c>
       <c r="D126" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="E126" t="s">
         <v>220</v>
@@ -9197,7 +9197,7 @@
         <v>443</v>
       </c>
       <c r="D127" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="E127" t="s">
         <v>18</v>
@@ -9226,7 +9226,7 @@
         <v>438</v>
       </c>
       <c r="D128" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="E128" t="s">
         <v>18</v>
@@ -9371,7 +9371,7 @@
         <v>446</v>
       </c>
       <c r="D133" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E133" t="s">
         <v>18</v>
@@ -9429,7 +9429,7 @@
         <v>435</v>
       </c>
       <c r="D135" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="E135" t="s">
         <v>18</v>
@@ -9458,7 +9458,7 @@
         <v>435</v>
       </c>
       <c r="D136" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="E136" t="s">
         <v>18</v>
@@ -9516,7 +9516,7 @@
         <v>436</v>
       </c>
       <c r="D138" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E138" t="s">
         <v>220</v>
@@ -9545,7 +9545,7 @@
         <v>84</v>
       </c>
       <c r="D139" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E139" t="s">
         <v>18</v>
@@ -9806,7 +9806,7 @@
         <v>444</v>
       </c>
       <c r="D148" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E148" t="s">
         <v>18</v>
@@ -9864,7 +9864,7 @@
         <v>435</v>
       </c>
       <c r="D150" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="E150" t="s">
         <v>18</v>
@@ -9893,7 +9893,7 @@
         <v>435</v>
       </c>
       <c r="D151" t="s">
-        <v>458</v>
+        <v>474</v>
       </c>
       <c r="E151" t="s">
         <v>18</v>
@@ -9951,7 +9951,7 @@
         <v>436</v>
       </c>
       <c r="D153" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="E153" t="s">
         <v>220</v>
@@ -9980,7 +9980,7 @@
         <v>84</v>
       </c>
       <c r="D154" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="E154" t="s">
         <v>18</v>
@@ -10009,7 +10009,7 @@
         <v>435</v>
       </c>
       <c r="D155" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="E155" t="s">
         <v>18</v>
@@ -10212,7 +10212,7 @@
         <v>444</v>
       </c>
       <c r="D162" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E162" t="s">
         <v>18</v>
@@ -10734,7 +10734,7 @@
         <v>449</v>
       </c>
       <c r="D180" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E180" t="s">
         <v>18</v>
@@ -10879,7 +10879,7 @@
         <v>449</v>
       </c>
       <c r="D185" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="E185" t="s">
         <v>18</v>

</xml_diff>